<commit_message>
Updated all except trade
</commit_message>
<xml_diff>
--- a/data-raw/NT/Forecasts.xlsx
+++ b/data-raw/NT/Forecasts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="47">
   <si>
     <t>Source</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>2024/25</t>
+  </si>
+  <si>
+    <t>2025/26</t>
   </si>
 </sst>
 </file>
@@ -452,6 +455,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1349,7 +1353,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1359,6 +1363,8 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="373">
     <cellStyle name="20% - Accent1 2" xfId="40"/>
@@ -2011,13 +2017,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y268"/>
+  <dimension ref="A1:Z283"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I236" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W255" sqref="W255"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,9 +2037,10 @@
     <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="25" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2109,8 +2116,11 @@
       <c r="Y1" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2152,7 +2162,7 @@
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2194,7 +2204,7 @@
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2236,7 +2246,7 @@
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2278,7 +2288,7 @@
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2320,7 +2330,7 @@
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2362,7 +2372,7 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2404,7 +2414,7 @@
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -2446,7 +2456,7 @@
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -2488,7 +2498,7 @@
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -2530,7 +2540,7 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -2572,7 +2582,7 @@
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -2614,7 +2624,7 @@
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -2656,7 +2666,7 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -2698,7 +2708,7 @@
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -12730,7 +12740,7 @@
         <v>286096.86099999998</v>
       </c>
     </row>
-    <row r="257" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>3</v>
       </c>
@@ -12756,7 +12766,7 @@
         <v>24099.151000000002</v>
       </c>
     </row>
-    <row r="258" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>3</v>
       </c>
@@ -12782,7 +12792,7 @@
         <v>22787.474999999999</v>
       </c>
     </row>
-    <row r="259" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>3</v>
       </c>
@@ -12808,7 +12818,7 @@
         <v>685483.11100000003</v>
       </c>
     </row>
-    <row r="260" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>3</v>
       </c>
@@ -12834,7 +12844,7 @@
         <v>505006.64799999999</v>
       </c>
     </row>
-    <row r="261" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>3</v>
       </c>
@@ -12860,7 +12870,7 @@
         <v>71272.414999999994</v>
       </c>
     </row>
-    <row r="262" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>3</v>
       </c>
@@ -12886,7 +12896,7 @@
         <v>1807613.835</v>
       </c>
     </row>
-    <row r="263" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>3</v>
       </c>
@@ -12912,7 +12922,7 @@
         <v>32013.195</v>
       </c>
     </row>
-    <row r="264" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>3</v>
       </c>
@@ -12938,7 +12948,7 @@
         <v>-65452.608</v>
       </c>
     </row>
-    <row r="265" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>3</v>
       </c>
@@ -12964,7 +12974,7 @@
         <v>1774174.423</v>
       </c>
     </row>
-    <row r="266" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>3</v>
       </c>
@@ -12977,20 +12987,20 @@
       <c r="D266" s="4">
         <v>13</v>
       </c>
-      <c r="V266" s="1">
+      <c r="V266" s="5">
         <v>0.247</v>
       </c>
-      <c r="W266" s="1">
+      <c r="W266" s="5">
         <v>0.248</v>
       </c>
-      <c r="X266" s="1">
+      <c r="X266" s="5">
         <v>0.249</v>
       </c>
-      <c r="Y266" s="1">
+      <c r="Y266" s="5">
         <v>0.25</v>
       </c>
     </row>
-    <row r="267" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>3</v>
       </c>
@@ -13016,7 +13026,7 @@
         <v>7233.7160000000003</v>
       </c>
     </row>
-    <row r="268" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>3</v>
       </c>
@@ -13040,6 +13050,396 @@
       </c>
       <c r="Y268" s="5">
         <v>1.0629999999999999</v>
+      </c>
+    </row>
+    <row r="269" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A269" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B269" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D269" s="2">
+        <v>1</v>
+      </c>
+      <c r="W269" s="7">
+        <v>989877</v>
+      </c>
+      <c r="X269" s="7">
+        <v>1021213</v>
+      </c>
+      <c r="Y269" s="7">
+        <v>1089123</v>
+      </c>
+      <c r="Z269" s="7">
+        <v>1172033</v>
+      </c>
+    </row>
+    <row r="270" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A270" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B270" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D270" s="2">
+        <v>2</v>
+      </c>
+      <c r="W270" s="7">
+        <v>601649</v>
+      </c>
+      <c r="X270" s="7">
+        <v>640300</v>
+      </c>
+      <c r="Y270" s="7">
+        <v>696624</v>
+      </c>
+      <c r="Z270" s="7">
+        <v>752627</v>
+      </c>
+    </row>
+    <row r="271" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B271" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D271" s="2">
+        <v>3</v>
+      </c>
+      <c r="W271" s="7">
+        <v>344944</v>
+      </c>
+      <c r="X271" s="7">
+        <v>336119</v>
+      </c>
+      <c r="Y271" s="7">
+        <v>345434</v>
+      </c>
+      <c r="Z271" s="7">
+        <v>369477</v>
+      </c>
+    </row>
+    <row r="272" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A272" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B272" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D272" s="2">
+        <v>4</v>
+      </c>
+      <c r="W272" s="7">
+        <v>21238</v>
+      </c>
+      <c r="X272" s="7">
+        <v>23027</v>
+      </c>
+      <c r="Y272" s="7">
+        <v>24816</v>
+      </c>
+      <c r="Z272" s="7">
+        <v>26846</v>
+      </c>
+    </row>
+    <row r="273" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A273" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B273" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D273" s="2">
+        <v>5</v>
+      </c>
+      <c r="W273" s="7">
+        <v>22656</v>
+      </c>
+      <c r="X273" s="7">
+        <v>23863</v>
+      </c>
+      <c r="Y273" s="7">
+        <v>25384</v>
+      </c>
+      <c r="Z273" s="7">
+        <v>27040</v>
+      </c>
+    </row>
+    <row r="274" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B274" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C274" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D274" s="4">
+        <v>6</v>
+      </c>
+      <c r="W274" s="7">
+        <v>581871</v>
+      </c>
+      <c r="X274" s="7">
+        <v>642765</v>
+      </c>
+      <c r="Y274" s="7">
+        <v>687208</v>
+      </c>
+      <c r="Z274" s="7">
+        <v>731032</v>
+      </c>
+    </row>
+    <row r="275" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A275" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B275" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D275" s="4">
+        <v>7</v>
+      </c>
+      <c r="W275" s="7">
+        <v>426283</v>
+      </c>
+      <c r="X275" s="7">
+        <v>471477</v>
+      </c>
+      <c r="Y275" s="7">
+        <v>505409</v>
+      </c>
+      <c r="Z275" s="7">
+        <v>537868</v>
+      </c>
+    </row>
+    <row r="276" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A276" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B276" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C276" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D276" s="4">
+        <v>8</v>
+      </c>
+      <c r="W276" s="7">
+        <v>76535</v>
+      </c>
+      <c r="X276" s="7">
+        <v>76588</v>
+      </c>
+      <c r="Y276" s="7">
+        <v>81195</v>
+      </c>
+      <c r="Z276" s="7">
+        <v>86506</v>
+      </c>
+    </row>
+    <row r="277" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A277" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B277" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D277" s="2">
+        <v>9</v>
+      </c>
+      <c r="W277" s="7">
+        <v>1692177</v>
+      </c>
+      <c r="X277" s="7">
+        <v>1787456</v>
+      </c>
+      <c r="Y277" s="7">
+        <v>1907727</v>
+      </c>
+      <c r="Z277" s="7">
+        <v>2043456</v>
+      </c>
+    </row>
+    <row r="278" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A278" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B278" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D278" s="2">
+        <v>10</v>
+      </c>
+      <c r="W278" s="7">
+        <v>55078</v>
+      </c>
+      <c r="X278" s="7">
+        <v>51583</v>
+      </c>
+      <c r="Y278" s="7">
+        <v>46859</v>
+      </c>
+      <c r="Z278" s="7">
+        <v>44310</v>
+      </c>
+    </row>
+    <row r="279" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A279" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B279" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D279" s="2">
+        <v>11</v>
+      </c>
+      <c r="W279" s="7">
+        <v>-43683</v>
+      </c>
+      <c r="X279" s="7">
+        <v>-79811</v>
+      </c>
+      <c r="Y279" s="7">
+        <v>-86505</v>
+      </c>
+      <c r="Z279" s="7">
+        <v>-80059</v>
+      </c>
+    </row>
+    <row r="280" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B280" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D280" s="2">
+        <v>12</v>
+      </c>
+      <c r="W280" s="7">
+        <v>1703571</v>
+      </c>
+      <c r="X280" s="7">
+        <v>1759229</v>
+      </c>
+      <c r="Y280" s="7">
+        <v>1868080</v>
+      </c>
+      <c r="Z280" s="7">
+        <v>2007707</v>
+      </c>
+    </row>
+    <row r="281" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A281" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B281" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C281" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D281" s="4">
+        <v>13</v>
+      </c>
+      <c r="W281" s="5">
+        <v>0.254</v>
+      </c>
+      <c r="X281" s="5">
+        <v>0.255</v>
+      </c>
+      <c r="Y281" s="5">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="Z281" s="5">
+        <v>0.25700000000000001</v>
+      </c>
+    </row>
+    <row r="282" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A282" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B282" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D282" s="4">
+        <v>14</v>
+      </c>
+      <c r="W282" s="8">
+        <v>6651.3</v>
+      </c>
+      <c r="X282" s="8">
+        <v>7005.7</v>
+      </c>
+      <c r="Y282" s="8">
+        <v>7452.4</v>
+      </c>
+      <c r="Z282" s="8">
+        <v>7938.5</v>
+      </c>
+    </row>
+    <row r="283" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A283" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B283" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D283" s="4">
+        <v>15</v>
+      </c>
+      <c r="W283" s="6">
+        <v>1.42</v>
+      </c>
+      <c r="X283" s="6">
+        <v>1.06</v>
+      </c>
+      <c r="Y283" s="6">
+        <v>1.06</v>
+      </c>
+      <c r="Z283" s="6">
+        <v>1.0900000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>